<commit_message>
conclusions are being written
</commit_message>
<xml_diff>
--- a/exports/apgar5unhealthy.xlsx
+++ b/exports/apgar5unhealthy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,223 +482,217 @@
       <c r="C2" t="n">
         <v>7.14</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
-        </is>
+      <c r="D2" t="n">
+        <v>13.10423286807256</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.025939589265073</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.37347590611476</v>
+      </c>
+      <c r="G2" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>1172</t>
+          <t>1065</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>7.12</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
-        </is>
+        <v>7.13</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22.29447150050382</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.626556528030944</v>
+      </c>
+      <c r="F3" t="n">
+        <v>14.58340096931597</v>
+      </c>
+      <c r="G3" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>1370</t>
+          <t>1172</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>7.03</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
-        </is>
+        <v>7.12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>11.43705331809856</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.920757794620315</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.20277796320079</v>
+      </c>
+      <c r="G4" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>1392</t>
+          <t>1370</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>7.26</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
-        </is>
+        <v>7.03</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10.64927355675065</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.7650142517193413</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.006603063537734</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>1399</t>
+          <t>1392</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>7.28</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
-        </is>
+        <v>7.26</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16.02409046434199</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.174723496625334</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.040278558458219</v>
+      </c>
+      <c r="G6" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>1406</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>7.07</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
-        </is>
+        <v>7.28</v>
+      </c>
+      <c r="D7" t="n">
+        <v>8.113389967505748</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.396139937127157</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.685676507111217</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>1404</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="D8" t="n">
+        <v>19.11824566937721</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.6266717308582</v>
+      </c>
+      <c r="F8" t="n">
+        <v>13.57207349789775</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>1406</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7.07</v>
+      </c>
+      <c r="D9" t="n">
+        <v>16.03109597208861</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.206187332209771</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7.832334238509944</v>
+      </c>
+      <c r="G9" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>1412</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
         <v>7.2</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
-        </is>
+      <c r="D10" t="n">
+        <v>18.04385261486464</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.155559826166355</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6.328767076480719</v>
+      </c>
+      <c r="G10" t="n">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>